<commit_message>
updated with distortion and wawa
</commit_message>
<xml_diff>
--- a/id dictatorship.xlsx
+++ b/id dictatorship.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>filterid</t>
   </si>
@@ -87,19 +87,13 @@
     <t>on/off</t>
   </si>
   <si>
-    <t>range or off</t>
-  </si>
-  <si>
-    <t>blend</t>
-  </si>
-  <si>
     <t>range</t>
   </si>
   <si>
     <t>wawa</t>
   </si>
   <si>
-    <t>gauchissement</t>
+    <t>distortion</t>
   </si>
 </sst>
 </file>
@@ -143,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,6 +146,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -451,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -463,7 +460,7 @@
     <col min="3" max="3" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -474,144 +471,141 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
@@ -620,7 +614,7 @@
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
@@ -629,7 +623,7 @@
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
@@ -638,8 +632,8 @@
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
+      <c r="B19" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>23</v>
@@ -649,7 +643,7 @@
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -660,27 +654,45 @@
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>26</v>
+      <c r="B22" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="2"/>
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:C5"/>

</xml_diff>

<commit_message>
Made WahWah SPI ready, added on/off feature SPI for distortion, updated id list of spi
</commit_message>
<xml_diff>
--- a/id dictatorship.xlsx
+++ b/id dictatorship.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bagas Prabowo\Documents\ouisician\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="14295" windowHeight="4890"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>filterid</t>
   </si>
@@ -87,9 +92,6 @@
     <t>on/off</t>
   </si>
   <si>
-    <t>range or off</t>
-  </si>
-  <si>
     <t>blend</t>
   </si>
   <si>
@@ -100,13 +102,16 @@
   </si>
   <si>
     <t>gauchissement</t>
+  </si>
+  <si>
+    <t>Range</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,19 +162,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -207,9 +226,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -241,9 +260,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +312,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -450,20 +505,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -474,213 +529,231 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>26</v>
+      <c r="B22" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:C5"/>
@@ -693,24 +766,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>